<commit_message>
intermediate commit. Table transfer part 2 is halfway done.
</commit_message>
<xml_diff>
--- a/cv_to_excel/demo.xlsx
+++ b/cv_to_excel/demo.xlsx
@@ -13,23 +13,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>World</t>
-  </si>
-  <si>
-    <t>Merged Range</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -37,38 +23,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -76,31 +40,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,70 +340,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="200.7109375" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="168.7109375" customWidth="1"/>
+    <col min="4" max="4" width="74.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
+    <row r="1" ht="27" customHeight="1"/>
+    <row r="2" ht="39" customHeight="1"/>
+    <row r="3" ht="17" customHeight="1"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B4:E9"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
intermediate commit 3. It's almost working - I'd say 95 percent
</commit_message>
<xml_diff>
--- a/cv_to_excel/demo.xlsx
+++ b/cv_to_excel/demo.xlsx
@@ -340,21 +340,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="168.7109375" customWidth="1"/>
-    <col min="4" max="4" width="74.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="8" max="8" width="55.7109375" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" customWidth="1"/>
+    <col min="10" max="10" width="65.7109375" customWidth="1"/>
+    <col min="11" max="11" width="70.7109375" customWidth="1"/>
+    <col min="12" max="12" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1"/>
-    <row r="2" ht="39" customHeight="1"/>
-    <row r="3" ht="17" customHeight="1"/>
+    <row r="1" ht="30" customHeight="1"/>
+    <row r="2" ht="40" customHeight="1"/>
+    <row r="3" ht="50" customHeight="1"/>
+    <row r="4" ht="60" customHeight="1"/>
+    <row r="5" ht="70" customHeight="1"/>
+    <row r="6" ht="80" customHeight="1"/>
+    <row r="7" ht="90" customHeight="1"/>
+    <row r="8" ht="100" customHeight="1"/>
+    <row r="9" ht="110" customHeight="1"/>
+    <row r="10" ht="120" customHeight="1"/>
+    <row r="11" ht="130" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
final commit for now. The functionality for this module is complete - the out function takes in a list of column widths and row heights and manipulates an excel file accordingly. It then writes data from a list of values containing merged/single cells and their corresponding data. 197 lines of code produced from 4 hours of hard work and brain cell loss.
</commit_message>
<xml_diff>
--- a/cv_to_excel/demo.xlsx
+++ b/cv_to_excel/demo.xlsx
@@ -11,6 +11,20 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>First entry</t>
+  </si>
+  <si>
+    <t>Second entry</t>
+  </si>
+  <si>
+    <t>second merge</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44,8 +58,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,18 +377,52 @@
     <col min="12" max="12" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1"/>
-    <row r="2" ht="40" customHeight="1"/>
-    <row r="3" ht="50" customHeight="1"/>
-    <row r="4" ht="60" customHeight="1"/>
-    <row r="5" ht="70" customHeight="1"/>
-    <row r="6" ht="80" customHeight="1"/>
-    <row r="7" ht="90" customHeight="1"/>
-    <row r="8" ht="100" customHeight="1"/>
-    <row r="9" ht="110" customHeight="1"/>
-    <row r="10" ht="120" customHeight="1"/>
-    <row r="11" ht="130" customHeight="1"/>
+    <row r="1" spans="1:6" ht="30" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="40" customHeight="1">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="50" customHeight="1">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="60" customHeight="1">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="70" customHeight="1">
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="80" customHeight="1"/>
+    <row r="7" spans="1:6" ht="90" customHeight="1">
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="100" customHeight="1">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="110" customHeight="1"/>
+    <row r="10" spans="1:6" ht="120" customHeight="1"/>
+    <row r="11" spans="1:6" ht="130" customHeight="1"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C4"/>
+    <mergeCell ref="E7:F8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
i lied... This is the ACTUAL last commit for a while. Everything's been put into 1 method and a slight modification was made because of a miscommunication of method argument formats.
</commit_message>
<xml_diff>
--- a/cv_to_excel/demo.xlsx
+++ b/cv_to_excel/demo.xlsx
@@ -383,21 +383,25 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="40" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="50" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="60" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="70" customHeight="1">
       <c r="D5" s="1" t="s">
@@ -420,7 +424,7 @@
     <row r="11" spans="1:6" ht="130" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:C4"/>
+    <mergeCell ref="A1:D4"/>
     <mergeCell ref="E7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>